<commit_message>
Initialization functional... products are successfully added to queues... config file successfully read...
</commit_message>
<xml_diff>
--- a/Project_3/Data/Config.xlsx
+++ b/Project_3/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\Uipath Processes\Pot_Alavrez_HansenProj3\Project_3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F59FCAB-AC57-4C94-885B-031007D375E2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2F6B92-A6B6-47C9-903B-90627164D87F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -153,55 +153,61 @@
     <t>Static part of logging message. Processed Transaction failed with application exception</t>
   </si>
   <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>logF_BusinessProcessName</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>cCardType</t>
+  </si>
+  <si>
+    <t>cCardExpiryMonth</t>
+  </si>
+  <si>
+    <t>cCardExpiryYear</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>C:\revature\Uipath Processes\Pot_Alavrez_HansenProj3\Project_3\Data\Config.xlsx</t>
+  </si>
+  <si>
+    <t>http://training.openspan.com/login</t>
+  </si>
+  <si>
+    <t>OrderProductsQueue</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
-    <t>KibanaDemoQueue</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
-    <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
-  </si>
-  <si>
-    <t>cCardType</t>
-  </si>
-  <si>
-    <t>cCardExpiryMonth</t>
-  </si>
-  <si>
-    <t>cCardExpiryYear</t>
-  </si>
-  <si>
-    <t>filePath</t>
-  </si>
-  <si>
-    <t>url</t>
-  </si>
-  <si>
-    <t>browser</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>Visa</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>C:\revature\Uipath Processes\Pot_Alavrez_HansenProj3\Project_3\Data\Config.xlsx</t>
-  </si>
-  <si>
-    <t>http://training.openspan.com/login</t>
+    <t>OrchestratorURL</t>
+  </si>
+  <si>
+    <t>https://demo.uipath.com/</t>
+  </si>
+  <si>
+    <t>Firefox</t>
   </si>
 </sst>
 </file>
@@ -560,7 +566,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -606,25 +614,32 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1629,7 +1644,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2842,7 +2859,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2888,23 +2905,23 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>2020</v>
@@ -2912,26 +2929,26 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
modified config.pdg to be a true JSON file and amended process accordingly... fixed bug with 'chopping' queueing technique...
</commit_message>
<xml_diff>
--- a/Project_3/Data/Config.xlsx
+++ b/Project_3/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revature\Uipath Processes\Pot_Alavrez_HansenProj3\Project_3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2F6B92-A6B6-47C9-903B-90627164D87F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0BE3A8-9F99-470F-8B18-EAD80FC8F565}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>http://training.openspan.com/login</t>
   </si>
   <si>
-    <t>OrderProductsQueue</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Firefox</t>
+  </si>
+  <si>
+    <t>PreOrder</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -614,10 +614,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
         <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2858,7 +2858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2948,7 +2948,7 @@
         <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>